<commit_message>
- As sent to manufacture on 13.12.2021
</commit_message>
<xml_diff>
--- a/docu/esp32_lolin_clone.xlsx
+++ b/docu/esp32_lolin_clone.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="132">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">MANUFACTURER_REF</t>
   </si>
   <si>
+    <t xml:space="preserve">REPLACEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">10K</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
     <t xml:space="preserve">Guangdong Hottech</t>
   </si>
   <si>
+    <t xml:space="preserve">WHITE</t>
+  </si>
+  <si>
     <t xml:space="preserve">LEDCHIP-LED0603</t>
   </si>
   <si>
@@ -347,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">Amphenol ICC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCSC: C2681556</t>
   </si>
   <si>
     <t xml:space="preserve">1X16_SMALLPAD</t>
@@ -421,6 +430,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -442,6 +452,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -511,7 +522,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,16 +603,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.07"/>
@@ -609,7 +620,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="25.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.36"/>
   </cols>
   <sheetData>
@@ -644,37 +655,40 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,31 +696,31 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,31 +728,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,63 +760,63 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="E6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="G6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>38</v>
+      <c r="J6" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,124 +824,127 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="H8" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>44</v>
+      <c r="I8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="C10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="E10" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="F10" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="G10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>64</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,63 +952,63 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="C12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="E12" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="F12" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="G12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,63 +1016,63 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="B14" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="C14" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="F14" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="G14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>90</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,63 +1080,63 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="C16" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="E16" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="F16" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="G16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>102</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,63 +1144,66 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="K17" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="B18" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="C18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>113</v>
+      <c r="E18" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,63 +1211,63 @@
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="H19" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="B20" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="C20" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="3" t="n">
+      <c r="E20" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" s="0" t="n">
         <v>9492615</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>117</v>
+      <c r="I20" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,31 +1275,31 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>